<commit_message>
add buffered benchmark result
</commit_message>
<xml_diff>
--- a/benchmark-4-16/benchmark_result.xlsx
+++ b/benchmark-4-16/benchmark_result.xlsx
@@ -11,7 +11,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+  <si>
+    <t>Unbuffered</t>
+  </si>
+  <si>
+    <t>Buffered</t>
+  </si>
   <si>
     <t>Program name</t>
   </si>
@@ -46,6 +52,15 @@
     <t>1.476s</t>
   </si>
   <si>
+    <t>0.670s</t>
+  </si>
+  <si>
+    <t>1.420s</t>
+  </si>
+  <si>
+    <t>1.452s</t>
+  </si>
+  <si>
     <t>a_simple_macro2</t>
   </si>
   <si>
@@ -61,6 +76,15 @@
     <t>29.709s</t>
   </si>
   <si>
+    <t>10.290s</t>
+  </si>
+  <si>
+    <t>11.481s</t>
+  </si>
+  <si>
+    <t>11.461s</t>
+  </si>
+  <si>
     <t>e_simple_macro</t>
   </si>
   <si>
@@ -73,6 +97,15 @@
     <t>1.428s</t>
   </si>
   <si>
+    <t>0.557s</t>
+  </si>
+  <si>
+    <t>1.477s</t>
+  </si>
+  <si>
+    <t>1.436s</t>
+  </si>
+  <si>
     <t>e_simple_macro2</t>
   </si>
   <si>
@@ -88,6 +121,15 @@
     <t>1.431s</t>
   </si>
   <si>
+    <t>0.500s</t>
+  </si>
+  <si>
+    <t>1.472s</t>
+  </si>
+  <si>
+    <t>1.445s</t>
+  </si>
+  <si>
     <t>e_simple_macro3</t>
   </si>
   <si>
@@ -97,20 +139,27 @@
     <t>0.501s</t>
   </si>
   <si>
-    <t>1.445s</t>
-  </si>
-  <si>
     <t>1.408s</t>
+  </si>
+  <si>
+    <t>0.488s</t>
+  </si>
+  <si>
+    <t>1.467s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font/>
@@ -169,23 +218,26 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -407,124 +459,186 @@
     <col customWidth="1" min="1" max="1" width="17.0"/>
   </cols>
   <sheetData>
+    <row r="1">
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="D2" s="2" t="s">
         <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="3">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4">
         <v>500.0</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="3">
+      <c r="A4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="4">
         <v>1.0E7</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>15</v>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="3">
+      <c r="A5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="4">
         <v>50.0</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>19</v>
+      <c r="C5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="3">
+      <c r="A6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="4">
         <v>5000.0</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>24</v>
+      <c r="C6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="5">
+      <c r="A7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="6">
         <v>100.0</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="C7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>